<commit_message>
added november  month update
</commit_message>
<xml_diff>
--- a/data/ISIMM_2019.xlsx
+++ b/data/ISIMM_2019.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6303" uniqueCount="1513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6303" uniqueCount="1496">
   <si>
     <t>PCODE</t>
   </si>
@@ -3928,255 +3928,102 @@
     <t>CP000704</t>
   </si>
   <si>
-    <t>Aleppo/حلب</t>
-  </si>
-  <si>
-    <t>Jebel Saman/جبل سمعان</t>
-  </si>
-  <si>
-    <t>Atareb/ أتارب</t>
-  </si>
-  <si>
-    <t>Al Saqiah * / الساقية</t>
-  </si>
-  <si>
     <t>CP000671</t>
   </si>
   <si>
-    <t>Mezanaz/ميزناز</t>
-  </si>
-  <si>
-    <t>abu baker al-seddiq*/ أبو بكر الصديق</t>
-  </si>
-  <si>
     <t>CP000672</t>
   </si>
   <si>
-    <t>Hamdo Aljasem*/ حمدو الجاسم</t>
-  </si>
-  <si>
     <t>CP000707</t>
   </si>
   <si>
-    <t>Al Waleed (Mezanaz) * / الوليد (ميزناز)</t>
-  </si>
-  <si>
     <t>CP000712</t>
   </si>
   <si>
-    <t>Jeineh/الجينة</t>
-  </si>
-  <si>
-    <t>Al Malaab (Jeineh) * / الملعب (الجينة)</t>
-  </si>
-  <si>
     <t>CP000673</t>
   </si>
   <si>
-    <t>Abin Samaan/ابين سمعان</t>
-  </si>
-  <si>
-    <t>Azeez */ مخيم عزيز</t>
-  </si>
-  <si>
     <t>CP000674</t>
   </si>
   <si>
-    <t>Zarbah/الزربة</t>
-  </si>
-  <si>
-    <t>Zarbah poultry*/ دواجن الزربة</t>
-  </si>
-  <si>
     <t>CP000705</t>
   </si>
   <si>
-    <t>Al Bo Assi * / البو عاصي</t>
-  </si>
-  <si>
     <t>CP000675</t>
   </si>
   <si>
-    <t>Kassibeh/كسيبة</t>
-  </si>
-  <si>
-    <t>Al_Ksaibh*/الكسيبة</t>
-  </si>
-  <si>
     <t>CP000676</t>
   </si>
   <si>
-    <t>Bawabiyeh/بوابية</t>
-  </si>
-  <si>
-    <t>Bawabia */بدوية</t>
-  </si>
-  <si>
     <t>CP000706</t>
   </si>
   <si>
-    <t>Mikman * / مكمان</t>
-  </si>
-  <si>
     <t>CP000677</t>
   </si>
   <si>
-    <t>Arada/عرادة</t>
-  </si>
-  <si>
-    <t>Beidar/ البيدر</t>
-  </si>
-  <si>
     <t>CP000678</t>
   </si>
   <si>
-    <t>EL-Iman/ الإيمان</t>
-  </si>
-  <si>
     <t>CP000679</t>
   </si>
   <si>
-    <t>Majbal / المجبل</t>
-  </si>
-  <si>
     <t>CP000680</t>
   </si>
   <si>
-    <t>Mashtal/ المشتل</t>
-  </si>
-  <si>
     <t>CP000681</t>
   </si>
   <si>
-    <t>Daret Azza/دارة عزة</t>
-  </si>
-  <si>
-    <t>Ebad Al_Rahman*/ عباد الرحمن</t>
-  </si>
-  <si>
     <t>CP000700</t>
   </si>
   <si>
-    <t>Idleb/إدلب</t>
-  </si>
-  <si>
-    <t>Harim/حارم</t>
-  </si>
-  <si>
-    <t>Dana/ دانا</t>
-  </si>
-  <si>
-    <t>Halap labeih */ حلب لبيه</t>
-  </si>
-  <si>
     <t>CP000655</t>
   </si>
   <si>
-    <t>Qah/ قاح</t>
-  </si>
-  <si>
-    <t>Shohadaa Alghab */ شهداء الغاب</t>
-  </si>
-  <si>
     <t>CP000666</t>
   </si>
   <si>
-    <t>Al Akram*/الأكرم</t>
-  </si>
-  <si>
     <t>CP000667</t>
   </si>
   <si>
-    <t>Wadi Alghazal*/وادي الغزال</t>
-  </si>
-  <si>
     <t>CP000656</t>
   </si>
   <si>
-    <t>Kafr Deryan/كفردريان</t>
-  </si>
-  <si>
-    <t>Kafr Deryan Camp*/ مخيم كفر دريان</t>
-  </si>
-  <si>
     <t>CP000687</t>
   </si>
   <si>
-    <t>Al Kalamoun*/ القلمون</t>
-  </si>
-  <si>
     <t>CP000660</t>
   </si>
   <si>
-    <t>Sarmada/ سرمدا</t>
-  </si>
-  <si>
-    <t>khaa Homs*/ إخاء حمص</t>
-  </si>
-  <si>
     <t>CP000661</t>
   </si>
   <si>
-    <t>Basmet Amal*/ بسمة أمل</t>
-  </si>
-  <si>
     <t>CP000662</t>
   </si>
   <si>
-    <t>Faheel Alez*/ فحيل العز</t>
-  </si>
-  <si>
     <t>CP000663</t>
   </si>
   <si>
-    <t>Saad bin abi wakkas*/سعد بن ابي وقاص</t>
-  </si>
-  <si>
     <t>CP000664</t>
   </si>
   <si>
-    <t>Sinjar Kahrabaa*/ سنجار الكهرباء</t>
-  </si>
-  <si>
     <t>CP000682</t>
   </si>
   <si>
-    <t>Al Wafaa(Sarmada)*/ (الوفاء(سرمدا</t>
-  </si>
-  <si>
     <t>CP000696</t>
   </si>
   <si>
-    <t>Abo Bakr Alsedek(Sarmada)*/ أبو بكر الصديق (سرمدا)</t>
-  </si>
-  <si>
     <t>CP000697</t>
   </si>
   <si>
-    <t>Al Ansar * / الأنصار</t>
-  </si>
-  <si>
     <t>CP000698</t>
   </si>
   <si>
-    <t>Shorleen * / شورلين</t>
-  </si>
-  <si>
     <t>CP000699</t>
   </si>
   <si>
-    <t>Al Diaa 2 * / الضياء 2</t>
-  </si>
-  <si>
     <t>CP000665</t>
   </si>
   <si>
-    <t>Burj Elnumra/برج النمرة</t>
-  </si>
-  <si>
-    <t>Borj*/ البرج</t>
-  </si>
-  <si>
     <t>CP000658</t>
   </si>
   <si>
@@ -4195,192 +4042,75 @@
     <t>CP000701</t>
   </si>
   <si>
-    <t>Tilaada/تلعادة</t>
-  </si>
-  <si>
-    <t>Tilaada * /  تلعادة</t>
-  </si>
-  <si>
     <t>CP000702</t>
   </si>
   <si>
-    <t>Al Etisam */ الاعتصام</t>
-  </si>
-  <si>
     <t>CP000703</t>
   </si>
   <si>
-    <t>Al Hijra * / الهجرة</t>
-  </si>
-  <si>
     <t>CP000710</t>
   </si>
   <si>
-    <t>Armanaz/أرمناز</t>
-  </si>
-  <si>
-    <t>Ghafar/الغفر</t>
-  </si>
-  <si>
-    <t>Ghafar * / الغفر</t>
-  </si>
-  <si>
     <t>CP000711</t>
   </si>
   <si>
-    <t>Al Nouri (Armanaz) * / النوري(أرمناز)</t>
-  </si>
-  <si>
     <t>CP000685</t>
   </si>
   <si>
-    <t>Idleb/مركز إدلب</t>
-  </si>
-  <si>
-    <t>Kelly/كللي</t>
-  </si>
-  <si>
-    <t>Tajamouaa Alrahma*/ تجمع الرحمة</t>
-  </si>
-  <si>
     <t>CP000686</t>
   </si>
   <si>
-    <t>Al Faysal*/ الفيصل</t>
-  </si>
-  <si>
     <t>CP000657</t>
   </si>
   <si>
-    <t>Batenta/باتنته</t>
-  </si>
-  <si>
-    <t>Al Hawija* / الحويجة</t>
-  </si>
-  <si>
     <t>CP000668</t>
   </si>
   <si>
-    <t>Hazano/حزانو</t>
-  </si>
-  <si>
-    <t>West of Mansour washer*/غربي مغسلة منصور</t>
-  </si>
-  <si>
     <t>CP000669</t>
   </si>
   <si>
-    <t>Behind of Mansour Washer*/خلف مغسلة منصور</t>
-  </si>
-  <si>
     <t>CP000670</t>
   </si>
   <si>
-    <t>Almakbara Alshemaly*/ المقبرة الشمالي</t>
-  </si>
-  <si>
     <t>CP000688</t>
   </si>
   <si>
-    <t>Maaret Tamsrin/ معرة تمصرين</t>
-  </si>
-  <si>
-    <t>Maarbouna*/ معربونة</t>
-  </si>
-  <si>
     <t>CP000689</t>
   </si>
   <si>
-    <t>Shekh Bahr/الشيخ بحر</t>
-  </si>
-  <si>
-    <t>Al Karamah(Shekh Bahr)*/ الكرامة(الشيخ بحر)</t>
-  </si>
-  <si>
     <t>CP000690</t>
   </si>
   <si>
-    <t>Murin / مورين</t>
-  </si>
-  <si>
-    <t>Murin Caps*/ تجمع مخيمان مورين</t>
-  </si>
-  <si>
     <t>CP000691</t>
   </si>
   <si>
-    <t>Al Anwar (Maart Msrin)*/ الانوار(معرة مصرين)</t>
-  </si>
-  <si>
     <t>CP000692</t>
   </si>
   <si>
-    <t xml:space="preserve"> Kafrehmul/الكفر_كفريحمول</t>
-  </si>
-  <si>
-    <t>Robaa Aljour / ربع الجور</t>
-  </si>
-  <si>
     <t>CP000693</t>
   </si>
   <si>
-    <t>Al Job / الجب</t>
-  </si>
-  <si>
     <t>CP000694</t>
   </si>
   <si>
-    <t>Al Zeyara (Batenta) * / الزيارة(باتنته)</t>
-  </si>
-  <si>
     <t>CP000695</t>
   </si>
   <si>
-    <t>Al Abbas */ العباس</t>
-  </si>
-  <si>
     <t>CP000708</t>
   </si>
   <si>
-    <t>Sarmin/سرمين</t>
-  </si>
-  <si>
-    <t>Manhal Almiah * / منهل المياه</t>
-  </si>
-  <si>
     <t>CP000709</t>
   </si>
   <si>
-    <t>Ritco * / ريتكو</t>
-  </si>
-  <si>
     <t>C0000712</t>
   </si>
   <si>
-    <t>Al-Swagheih/الصواغية</t>
-  </si>
-  <si>
-    <t>Ahl Alkhair(Al Sawagheih) * / أهل الخير (الصواغية)</t>
-  </si>
-  <si>
     <t>CP000683</t>
   </si>
   <si>
-    <t>Jisr-Ash-Shugur/جسر الشغور</t>
-  </si>
-  <si>
-    <t>Jisr-Ash-Shugur/ جسر الشغور</t>
-  </si>
-  <si>
-    <t>Bayt Soufan*/ بيت صوفان</t>
-  </si>
-  <si>
     <t>CP000684</t>
   </si>
   <si>
-    <t>Kafilt Alkhair*/ قافلة الخير</t>
-  </si>
-  <si>
     <t>36.1085108,36.9300722</t>
   </si>
   <si>
@@ -4556,6 +4286,225 @@
   </si>
   <si>
     <t>35.947949,36.205759</t>
+  </si>
+  <si>
+    <t>Al Nouri (Armanaz)</t>
+  </si>
+  <si>
+    <t>Abin Samaan</t>
+  </si>
+  <si>
+    <t>Azeez</t>
+  </si>
+  <si>
+    <t>Ahl Alkhair(Al Sawagheih)</t>
+  </si>
+  <si>
+    <t>Al-Swagheih</t>
+  </si>
+  <si>
+    <t>Beidar</t>
+  </si>
+  <si>
+    <t>EL-Iman</t>
+  </si>
+  <si>
+    <t>khaa Homs</t>
+  </si>
+  <si>
+    <t>Basmet Amal</t>
+  </si>
+  <si>
+    <t>Faheel Alez</t>
+  </si>
+  <si>
+    <t>Saad bin abi wakkas</t>
+  </si>
+  <si>
+    <t>Sinjar Kahrabaa</t>
+  </si>
+  <si>
+    <t>Al Wafaa(Sarmada)</t>
+  </si>
+  <si>
+    <t>Abo Bakr Alsedek(Sarmada)</t>
+  </si>
+  <si>
+    <t>Al Ansar</t>
+  </si>
+  <si>
+    <t>Shorleen</t>
+  </si>
+  <si>
+    <t>Al Diaa 2</t>
+  </si>
+  <si>
+    <t>Zarbah</t>
+  </si>
+  <si>
+    <t>Shekh Bahr</t>
+  </si>
+  <si>
+    <t>Sarmin</t>
+  </si>
+  <si>
+    <t>Zarbah poultry</t>
+  </si>
+  <si>
+    <t>Al Bo Assi</t>
+  </si>
+  <si>
+    <t>Majbal</t>
+  </si>
+  <si>
+    <t>Mashtal</t>
+  </si>
+  <si>
+    <t>Al Karamah(Shekh Bahr)</t>
+  </si>
+  <si>
+    <t>Manhal Almiah</t>
+  </si>
+  <si>
+    <t>Tilaada</t>
+  </si>
+  <si>
+    <t>Murin</t>
+  </si>
+  <si>
+    <t>Murin Caps</t>
+  </si>
+  <si>
+    <t>Al Etisam</t>
+  </si>
+  <si>
+    <t>Al Saqiah</t>
+  </si>
+  <si>
+    <t>Shohadaa Alghab</t>
+  </si>
+  <si>
+    <t>Al Akram</t>
+  </si>
+  <si>
+    <t>Wadi Alghazal</t>
+  </si>
+  <si>
+    <t>Bawabiyeh</t>
+  </si>
+  <si>
+    <t>Daret Azza</t>
+  </si>
+  <si>
+    <t>Burj Elnumra</t>
+  </si>
+  <si>
+    <t>Batenta</t>
+  </si>
+  <si>
+    <t>Bawabia</t>
+  </si>
+  <si>
+    <t>Mikman</t>
+  </si>
+  <si>
+    <t>Ebad Al_Rahman</t>
+  </si>
+  <si>
+    <t>Borj</t>
+  </si>
+  <si>
+    <t>Al Hawija</t>
+  </si>
+  <si>
+    <t>Al Zeyara (Batenta)</t>
+  </si>
+  <si>
+    <t>Mezanaz</t>
+  </si>
+  <si>
+    <t>Jeineh</t>
+  </si>
+  <si>
+    <t>Kassibeh</t>
+  </si>
+  <si>
+    <t>Kafr Deryan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kafrehmul</t>
+  </si>
+  <si>
+    <t>abu baker al-seddiq</t>
+  </si>
+  <si>
+    <t>Hamdo Aljasem</t>
+  </si>
+  <si>
+    <t>Al Waleed (Mezanaz)</t>
+  </si>
+  <si>
+    <t>Al Malaab (Jeineh)</t>
+  </si>
+  <si>
+    <t>Al_Ksaibh</t>
+  </si>
+  <si>
+    <t>Kafr Deryan Camp</t>
+  </si>
+  <si>
+    <t>Al Kalamoun</t>
+  </si>
+  <si>
+    <t>Maarbouna</t>
+  </si>
+  <si>
+    <t>Al Anwar (Maart Msrin)</t>
+  </si>
+  <si>
+    <t>Robaa Aljour</t>
+  </si>
+  <si>
+    <t>Al Job</t>
+  </si>
+  <si>
+    <t>Ritco</t>
+  </si>
+  <si>
+    <t>Halap labeih</t>
+  </si>
+  <si>
+    <t>Al Hijra</t>
+  </si>
+  <si>
+    <t>Ghafar</t>
+  </si>
+  <si>
+    <t>Hazano</t>
+  </si>
+  <si>
+    <t>West of Mansour washer</t>
+  </si>
+  <si>
+    <t>Behind of Mansour Washer</t>
+  </si>
+  <si>
+    <t>Almakbara Alshemaly</t>
+  </si>
+  <si>
+    <t>Al Abbas</t>
+  </si>
+  <si>
+    <t>Bayt Soufan</t>
+  </si>
+  <si>
+    <t>Kafilt Alkhair</t>
+  </si>
+  <si>
+    <t>Tajamouaa Alrahma</t>
+  </si>
+  <si>
+    <t>Al Faysal</t>
   </si>
 </sst>
 </file>
@@ -4903,16 +4852,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X484"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="43.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="55.33203125" customWidth="1"/>
     <col min="13" max="13" width="9.77734375" bestFit="1" customWidth="1"/>
@@ -35924,19 +35874,19 @@
         <v>1302</v>
       </c>
       <c r="B426" t="s">
-        <v>1303</v>
+        <v>24</v>
       </c>
       <c r="C426" t="s">
-        <v>1304</v>
+        <v>90</v>
       </c>
       <c r="D426" t="s">
-        <v>1305</v>
+        <v>91</v>
       </c>
       <c r="E426" t="s">
-        <v>1306</v>
+        <v>1453</v>
       </c>
       <c r="F426" t="s">
-        <v>1454</v>
+        <v>1364</v>
       </c>
       <c r="G426" t="s">
         <v>27</v>
@@ -35977,22 +35927,22 @@
     </row>
     <row r="427" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A427" s="2" t="s">
-        <v>1307</v>
+        <v>1303</v>
       </c>
       <c r="B427" t="s">
-        <v>1303</v>
+        <v>24</v>
       </c>
       <c r="C427" t="s">
-        <v>1304</v>
+        <v>90</v>
       </c>
       <c r="D427" t="s">
-        <v>1308</v>
+        <v>1467</v>
       </c>
       <c r="E427" t="s">
-        <v>1309</v>
+        <v>1472</v>
       </c>
       <c r="F427" t="s">
-        <v>1455</v>
+        <v>1365</v>
       </c>
       <c r="G427" t="s">
         <v>95</v>
@@ -36033,22 +35983,22 @@
     </row>
     <row r="428" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A428" s="2" t="s">
-        <v>1310</v>
+        <v>1304</v>
       </c>
       <c r="B428" t="s">
-        <v>1303</v>
+        <v>24</v>
       </c>
       <c r="C428" t="s">
-        <v>1304</v>
+        <v>90</v>
       </c>
       <c r="D428" t="s">
-        <v>1308</v>
+        <v>1467</v>
       </c>
       <c r="E428" t="s">
-        <v>1311</v>
+        <v>1473</v>
       </c>
       <c r="F428" t="s">
-        <v>1456</v>
+        <v>1366</v>
       </c>
       <c r="G428" t="s">
         <v>95</v>
@@ -36089,22 +36039,22 @@
     </row>
     <row r="429" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A429" s="2" t="s">
-        <v>1312</v>
+        <v>1305</v>
       </c>
       <c r="B429" t="s">
-        <v>1303</v>
+        <v>24</v>
       </c>
       <c r="C429" t="s">
-        <v>1304</v>
+        <v>90</v>
       </c>
       <c r="D429" t="s">
-        <v>1308</v>
+        <v>1467</v>
       </c>
       <c r="E429" t="s">
-        <v>1313</v>
+        <v>1474</v>
       </c>
       <c r="F429" t="s">
-        <v>1457</v>
+        <v>1367</v>
       </c>
       <c r="G429" t="s">
         <v>27</v>
@@ -36145,22 +36095,22 @@
     </row>
     <row r="430" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A430" s="2" t="s">
-        <v>1314</v>
+        <v>1306</v>
       </c>
       <c r="B430" t="s">
-        <v>1303</v>
+        <v>24</v>
       </c>
       <c r="C430" t="s">
-        <v>1304</v>
+        <v>90</v>
       </c>
       <c r="D430" t="s">
-        <v>1315</v>
+        <v>1468</v>
       </c>
       <c r="E430" t="s">
-        <v>1316</v>
+        <v>1475</v>
       </c>
       <c r="F430" t="s">
-        <v>1458</v>
+        <v>1368</v>
       </c>
       <c r="G430" t="s">
         <v>27</v>
@@ -36201,22 +36151,22 @@
     </row>
     <row r="431" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A431" s="2" t="s">
-        <v>1317</v>
+        <v>1307</v>
       </c>
       <c r="B431" t="s">
-        <v>1303</v>
+        <v>24</v>
       </c>
       <c r="C431" t="s">
-        <v>1304</v>
+        <v>90</v>
       </c>
       <c r="D431" t="s">
-        <v>1318</v>
+        <v>1424</v>
       </c>
       <c r="E431" t="s">
-        <v>1319</v>
+        <v>1425</v>
       </c>
       <c r="F431" t="s">
-        <v>1459</v>
+        <v>1369</v>
       </c>
       <c r="G431" t="s">
         <v>27</v>
@@ -36257,22 +36207,22 @@
     </row>
     <row r="432" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A432" s="2" t="s">
-        <v>1320</v>
+        <v>1308</v>
       </c>
       <c r="B432" t="s">
-        <v>1303</v>
+        <v>24</v>
       </c>
       <c r="C432" t="s">
-        <v>1304</v>
+        <v>90</v>
       </c>
       <c r="D432" t="s">
-        <v>1321</v>
+        <v>1440</v>
       </c>
       <c r="E432" t="s">
-        <v>1322</v>
+        <v>1443</v>
       </c>
       <c r="F432" t="s">
-        <v>1460</v>
+        <v>1370</v>
       </c>
       <c r="G432" t="s">
         <v>27</v>
@@ -36313,22 +36263,22 @@
     </row>
     <row r="433" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A433" s="2" t="s">
-        <v>1323</v>
+        <v>1309</v>
       </c>
       <c r="B433" t="s">
-        <v>1303</v>
+        <v>24</v>
       </c>
       <c r="C433" t="s">
-        <v>1304</v>
+        <v>90</v>
       </c>
       <c r="D433" t="s">
-        <v>1321</v>
+        <v>1440</v>
       </c>
       <c r="E433" t="s">
-        <v>1324</v>
+        <v>1444</v>
       </c>
       <c r="F433" t="s">
-        <v>1461</v>
+        <v>1371</v>
       </c>
       <c r="G433" t="s">
         <v>27</v>
@@ -36369,22 +36319,22 @@
     </row>
     <row r="434" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A434" s="2" t="s">
-        <v>1325</v>
+        <v>1310</v>
       </c>
       <c r="B434" t="s">
-        <v>1303</v>
+        <v>24</v>
       </c>
       <c r="C434" t="s">
-        <v>1304</v>
+        <v>90</v>
       </c>
       <c r="D434" t="s">
-        <v>1326</v>
+        <v>1469</v>
       </c>
       <c r="E434" t="s">
-        <v>1327</v>
+        <v>1476</v>
       </c>
       <c r="F434" t="s">
-        <v>1462</v>
+        <v>1372</v>
       </c>
       <c r="G434" t="s">
         <v>27</v>
@@ -36425,22 +36375,22 @@
     </row>
     <row r="435" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A435" s="2" t="s">
-        <v>1328</v>
+        <v>1311</v>
       </c>
       <c r="B435" t="s">
-        <v>1303</v>
+        <v>24</v>
       </c>
       <c r="C435" t="s">
-        <v>1304</v>
+        <v>90</v>
       </c>
       <c r="D435" t="s">
-        <v>1329</v>
+        <v>1457</v>
       </c>
       <c r="E435" t="s">
-        <v>1330</v>
+        <v>1461</v>
       </c>
       <c r="F435" t="s">
-        <v>1463</v>
+        <v>1373</v>
       </c>
       <c r="G435" t="s">
         <v>27</v>
@@ -36481,22 +36431,22 @@
     </row>
     <row r="436" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A436" s="2" t="s">
-        <v>1331</v>
+        <v>1312</v>
       </c>
       <c r="B436" t="s">
-        <v>1303</v>
+        <v>24</v>
       </c>
       <c r="C436" t="s">
-        <v>1304</v>
+        <v>90</v>
       </c>
       <c r="D436" t="s">
-        <v>1329</v>
+        <v>1457</v>
       </c>
       <c r="E436" t="s">
-        <v>1332</v>
+        <v>1462</v>
       </c>
       <c r="F436" t="s">
-        <v>1464</v>
+        <v>1374</v>
       </c>
       <c r="G436" t="s">
         <v>95</v>
@@ -36537,22 +36487,22 @@
     </row>
     <row r="437" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A437" s="2" t="s">
-        <v>1333</v>
+        <v>1313</v>
       </c>
       <c r="B437" t="s">
-        <v>1303</v>
+        <v>24</v>
       </c>
       <c r="C437" t="s">
-        <v>1304</v>
+        <v>90</v>
       </c>
       <c r="D437" t="s">
-        <v>1334</v>
+        <v>950</v>
       </c>
       <c r="E437" t="s">
-        <v>1335</v>
+        <v>1428</v>
       </c>
       <c r="F437" t="s">
-        <v>1465</v>
+        <v>1375</v>
       </c>
       <c r="G437" t="s">
         <v>27</v>
@@ -36593,22 +36543,22 @@
     </row>
     <row r="438" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A438" s="2" t="s">
-        <v>1336</v>
+        <v>1314</v>
       </c>
       <c r="B438" t="s">
-        <v>1303</v>
+        <v>24</v>
       </c>
       <c r="C438" t="s">
-        <v>1304</v>
+        <v>90</v>
       </c>
       <c r="D438" t="s">
-        <v>1334</v>
+        <v>950</v>
       </c>
       <c r="E438" t="s">
-        <v>1337</v>
+        <v>1429</v>
       </c>
       <c r="F438" t="s">
-        <v>1466</v>
+        <v>1376</v>
       </c>
       <c r="G438" t="s">
         <v>27</v>
@@ -36649,22 +36599,22 @@
     </row>
     <row r="439" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A439" s="2" t="s">
-        <v>1338</v>
+        <v>1315</v>
       </c>
       <c r="B439" t="s">
-        <v>1303</v>
+        <v>24</v>
       </c>
       <c r="C439" t="s">
-        <v>1304</v>
+        <v>90</v>
       </c>
       <c r="D439" t="s">
-        <v>1321</v>
+        <v>1440</v>
       </c>
       <c r="E439" t="s">
-        <v>1339</v>
+        <v>1445</v>
       </c>
       <c r="F439" t="s">
-        <v>1467</v>
+        <v>1377</v>
       </c>
       <c r="G439" t="s">
         <v>27</v>
@@ -36705,22 +36655,22 @@
     </row>
     <row r="440" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A440" s="2" t="s">
-        <v>1340</v>
+        <v>1316</v>
       </c>
       <c r="B440" t="s">
-        <v>1303</v>
+        <v>24</v>
       </c>
       <c r="C440" t="s">
-        <v>1304</v>
+        <v>90</v>
       </c>
       <c r="D440" t="s">
-        <v>1321</v>
+        <v>1440</v>
       </c>
       <c r="E440" t="s">
-        <v>1341</v>
+        <v>1446</v>
       </c>
       <c r="F440" t="s">
-        <v>1468</v>
+        <v>1378</v>
       </c>
       <c r="G440" t="s">
         <v>27</v>
@@ -36761,22 +36711,22 @@
     </row>
     <row r="441" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A441" s="2" t="s">
-        <v>1342</v>
+        <v>1317</v>
       </c>
       <c r="B441" t="s">
-        <v>1303</v>
+        <v>24</v>
       </c>
       <c r="C441" t="s">
-        <v>1304</v>
+        <v>90</v>
       </c>
       <c r="D441" t="s">
-        <v>1343</v>
+        <v>1458</v>
       </c>
       <c r="E441" t="s">
-        <v>1344</v>
+        <v>1463</v>
       </c>
       <c r="F441" t="s">
-        <v>1469</v>
+        <v>1379</v>
       </c>
       <c r="G441" t="s">
         <v>27</v>
@@ -36817,22 +36767,22 @@
     </row>
     <row r="442" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A442" s="2" t="s">
-        <v>1345</v>
+        <v>1318</v>
       </c>
       <c r="B442" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C442" t="s">
-        <v>1347</v>
+        <v>113</v>
       </c>
       <c r="D442" t="s">
-        <v>1348</v>
+        <v>280</v>
       </c>
       <c r="E442" t="s">
-        <v>1349</v>
+        <v>1484</v>
       </c>
       <c r="F442" t="s">
-        <v>1470</v>
+        <v>1380</v>
       </c>
       <c r="G442" t="s">
         <v>56</v>
@@ -36873,22 +36823,22 @@
     </row>
     <row r="443" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A443" s="2" t="s">
-        <v>1350</v>
+        <v>1319</v>
       </c>
       <c r="B443" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C443" t="s">
-        <v>1347</v>
+        <v>113</v>
       </c>
       <c r="D443" t="s">
-        <v>1351</v>
+        <v>473</v>
       </c>
       <c r="E443" t="s">
-        <v>1352</v>
+        <v>1454</v>
       </c>
       <c r="F443" t="s">
-        <v>1471</v>
+        <v>1381</v>
       </c>
       <c r="G443" t="s">
         <v>27</v>
@@ -36929,22 +36879,22 @@
     </row>
     <row r="444" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A444" s="2" t="s">
-        <v>1353</v>
+        <v>1320</v>
       </c>
       <c r="B444" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C444" t="s">
-        <v>1347</v>
+        <v>113</v>
       </c>
       <c r="D444" t="s">
-        <v>1351</v>
+        <v>473</v>
       </c>
       <c r="E444" t="s">
-        <v>1354</v>
+        <v>1455</v>
       </c>
       <c r="F444" t="s">
-        <v>1472</v>
+        <v>1382</v>
       </c>
       <c r="G444" t="s">
         <v>27</v>
@@ -36985,22 +36935,22 @@
     </row>
     <row r="445" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A445" s="2" t="s">
-        <v>1355</v>
+        <v>1321</v>
       </c>
       <c r="B445" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C445" t="s">
-        <v>1347</v>
+        <v>113</v>
       </c>
       <c r="D445" t="s">
-        <v>1351</v>
+        <v>473</v>
       </c>
       <c r="E445" t="s">
-        <v>1356</v>
+        <v>1456</v>
       </c>
       <c r="F445" t="s">
-        <v>1473</v>
+        <v>1383</v>
       </c>
       <c r="G445" t="s">
         <v>27</v>
@@ -37041,22 +36991,22 @@
     </row>
     <row r="446" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A446" s="2" t="s">
-        <v>1357</v>
+        <v>1322</v>
       </c>
       <c r="B446" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C446" t="s">
-        <v>1347</v>
+        <v>113</v>
       </c>
       <c r="D446" t="s">
-        <v>1358</v>
+        <v>1470</v>
       </c>
       <c r="E446" t="s">
-        <v>1359</v>
+        <v>1477</v>
       </c>
       <c r="F446" t="s">
-        <v>1474</v>
+        <v>1384</v>
       </c>
       <c r="G446" t="s">
         <v>27</v>
@@ -37097,22 +37047,22 @@
     </row>
     <row r="447" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A447" s="2" t="s">
-        <v>1360</v>
+        <v>1323</v>
       </c>
       <c r="B447" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C447" t="s">
-        <v>1347</v>
+        <v>113</v>
       </c>
       <c r="D447" t="s">
-        <v>1358</v>
+        <v>1470</v>
       </c>
       <c r="E447" t="s">
-        <v>1361</v>
+        <v>1478</v>
       </c>
       <c r="F447" t="s">
-        <v>1475</v>
+        <v>1385</v>
       </c>
       <c r="G447" t="s">
         <v>27</v>
@@ -37153,22 +37103,22 @@
     </row>
     <row r="448" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A448" s="2" t="s">
-        <v>1362</v>
+        <v>1324</v>
       </c>
       <c r="B448" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C448" t="s">
-        <v>1347</v>
+        <v>113</v>
       </c>
       <c r="D448" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="E448" t="s">
-        <v>1364</v>
+        <v>1430</v>
       </c>
       <c r="F448" t="s">
-        <v>1476</v>
+        <v>1386</v>
       </c>
       <c r="G448" t="s">
         <v>27</v>
@@ -37209,22 +37159,22 @@
     </row>
     <row r="449" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A449" s="2" t="s">
-        <v>1365</v>
+        <v>1325</v>
       </c>
       <c r="B449" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C449" t="s">
-        <v>1347</v>
+        <v>113</v>
       </c>
       <c r="D449" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="E449" t="s">
-        <v>1366</v>
+        <v>1431</v>
       </c>
       <c r="F449" t="s">
-        <v>1477</v>
+        <v>1387</v>
       </c>
       <c r="G449" t="s">
         <v>27</v>
@@ -37265,22 +37215,22 @@
     </row>
     <row r="450" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A450" s="2" t="s">
-        <v>1367</v>
+        <v>1326</v>
       </c>
       <c r="B450" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C450" t="s">
-        <v>1347</v>
+        <v>113</v>
       </c>
       <c r="D450" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="E450" t="s">
-        <v>1368</v>
+        <v>1432</v>
       </c>
       <c r="F450" t="s">
-        <v>1478</v>
+        <v>1388</v>
       </c>
       <c r="G450" t="s">
         <v>27</v>
@@ -37321,22 +37271,22 @@
     </row>
     <row r="451" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A451" s="2" t="s">
-        <v>1369</v>
+        <v>1327</v>
       </c>
       <c r="B451" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C451" t="s">
-        <v>1347</v>
+        <v>113</v>
       </c>
       <c r="D451" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="E451" t="s">
-        <v>1370</v>
+        <v>1433</v>
       </c>
       <c r="F451" t="s">
-        <v>1479</v>
+        <v>1389</v>
       </c>
       <c r="G451" t="s">
         <v>27</v>
@@ -37377,22 +37327,22 @@
     </row>
     <row r="452" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A452" s="2" t="s">
-        <v>1371</v>
+        <v>1328</v>
       </c>
       <c r="B452" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C452" t="s">
-        <v>1347</v>
+        <v>113</v>
       </c>
       <c r="D452" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="E452" t="s">
-        <v>1372</v>
+        <v>1434</v>
       </c>
       <c r="F452" t="s">
-        <v>1480</v>
+        <v>1390</v>
       </c>
       <c r="G452" t="s">
         <v>27</v>
@@ -37433,22 +37383,22 @@
     </row>
     <row r="453" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A453" s="2" t="s">
-        <v>1373</v>
+        <v>1329</v>
       </c>
       <c r="B453" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C453" t="s">
-        <v>1347</v>
+        <v>113</v>
       </c>
       <c r="D453" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="E453" t="s">
-        <v>1374</v>
+        <v>1435</v>
       </c>
       <c r="F453" t="s">
-        <v>1481</v>
+        <v>1391</v>
       </c>
       <c r="G453" t="s">
         <v>27</v>
@@ -37489,22 +37439,22 @@
     </row>
     <row r="454" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A454" s="2" t="s">
-        <v>1375</v>
+        <v>1330</v>
       </c>
       <c r="B454" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C454" t="s">
-        <v>1347</v>
+        <v>113</v>
       </c>
       <c r="D454" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="E454" t="s">
-        <v>1376</v>
+        <v>1436</v>
       </c>
       <c r="F454" t="s">
-        <v>1482</v>
+        <v>1392</v>
       </c>
       <c r="G454" t="s">
         <v>27</v>
@@ -37545,22 +37495,22 @@
     </row>
     <row r="455" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A455" s="2" t="s">
-        <v>1377</v>
+        <v>1331</v>
       </c>
       <c r="B455" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C455" t="s">
-        <v>1347</v>
+        <v>113</v>
       </c>
       <c r="D455" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="E455" t="s">
-        <v>1378</v>
+        <v>1437</v>
       </c>
       <c r="F455" t="s">
-        <v>1483</v>
+        <v>1393</v>
       </c>
       <c r="G455" t="s">
         <v>27</v>
@@ -37601,22 +37551,22 @@
     </row>
     <row r="456" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A456" s="2" t="s">
-        <v>1379</v>
+        <v>1332</v>
       </c>
       <c r="B456" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C456" t="s">
-        <v>1347</v>
+        <v>113</v>
       </c>
       <c r="D456" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="E456" t="s">
-        <v>1380</v>
+        <v>1438</v>
       </c>
       <c r="F456" t="s">
-        <v>1484</v>
+        <v>1394</v>
       </c>
       <c r="G456" t="s">
         <v>27</v>
@@ -37657,22 +37607,22 @@
     </row>
     <row r="457" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A457" s="2" t="s">
-        <v>1381</v>
+        <v>1333</v>
       </c>
       <c r="B457" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C457" t="s">
-        <v>1347</v>
+        <v>113</v>
       </c>
       <c r="D457" t="s">
-        <v>1363</v>
+        <v>606</v>
       </c>
       <c r="E457" t="s">
-        <v>1382</v>
+        <v>1439</v>
       </c>
       <c r="F457" t="s">
-        <v>1485</v>
+        <v>1395</v>
       </c>
       <c r="G457" t="s">
         <v>56</v>
@@ -37713,22 +37663,22 @@
     </row>
     <row r="458" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A458" s="2" t="s">
-        <v>1383</v>
+        <v>1334</v>
       </c>
       <c r="B458" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C458" t="s">
-        <v>1347</v>
+        <v>113</v>
       </c>
       <c r="D458" t="s">
-        <v>1384</v>
+        <v>1459</v>
       </c>
       <c r="E458" t="s">
-        <v>1385</v>
+        <v>1464</v>
       </c>
       <c r="F458" t="s">
-        <v>1486</v>
+        <v>1396</v>
       </c>
       <c r="G458" t="s">
         <v>27</v>
@@ -37769,22 +37719,22 @@
     </row>
     <row r="459" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A459" s="2" t="s">
-        <v>1386</v>
+        <v>1335</v>
       </c>
       <c r="B459" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C459" t="s">
-        <v>1347</v>
+        <v>113</v>
       </c>
       <c r="D459" t="s">
-        <v>1387</v>
+        <v>1336</v>
       </c>
       <c r="E459" t="s">
-        <v>1388</v>
+        <v>1337</v>
       </c>
       <c r="F459" t="s">
-        <v>1487</v>
+        <v>1397</v>
       </c>
       <c r="G459" t="s">
         <v>27</v>
@@ -37825,22 +37775,22 @@
     </row>
     <row r="460" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A460" s="2" t="s">
-        <v>1389</v>
+        <v>1338</v>
       </c>
       <c r="B460" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C460" t="s">
-        <v>1347</v>
+        <v>113</v>
       </c>
       <c r="D460" t="s">
-        <v>1387</v>
+        <v>1336</v>
       </c>
       <c r="E460" t="s">
-        <v>1390</v>
+        <v>1339</v>
       </c>
       <c r="F460" t="s">
-        <v>1488</v>
+        <v>1398</v>
       </c>
       <c r="G460" t="s">
         <v>27</v>
@@ -37881,22 +37831,22 @@
     </row>
     <row r="461" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A461" s="2" t="s">
-        <v>1391</v>
+        <v>1340</v>
       </c>
       <c r="B461" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C461" t="s">
-        <v>1347</v>
+        <v>113</v>
       </c>
       <c r="D461" t="s">
-        <v>1392</v>
+        <v>1449</v>
       </c>
       <c r="E461" t="s">
-        <v>1393</v>
+        <v>1449</v>
       </c>
       <c r="F461" t="s">
-        <v>1489</v>
+        <v>1399</v>
       </c>
       <c r="G461" t="s">
         <v>27</v>
@@ -37937,22 +37887,22 @@
     </row>
     <row r="462" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A462" s="2" t="s">
-        <v>1394</v>
+        <v>1341</v>
       </c>
       <c r="B462" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C462" t="s">
-        <v>1347</v>
+        <v>113</v>
       </c>
       <c r="D462" t="s">
-        <v>1392</v>
+        <v>1449</v>
       </c>
       <c r="E462" t="s">
-        <v>1395</v>
+        <v>1452</v>
       </c>
       <c r="F462" t="s">
-        <v>1490</v>
+        <v>1400</v>
       </c>
       <c r="G462" t="s">
         <v>27</v>
@@ -37993,22 +37943,22 @@
     </row>
     <row r="463" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A463" s="2" t="s">
-        <v>1396</v>
+        <v>1342</v>
       </c>
       <c r="B463" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C463" t="s">
-        <v>1347</v>
+        <v>113</v>
       </c>
       <c r="D463" t="s">
-        <v>1348</v>
+        <v>280</v>
       </c>
       <c r="E463" t="s">
-        <v>1397</v>
+        <v>1485</v>
       </c>
       <c r="F463" t="s">
-        <v>1491</v>
+        <v>1401</v>
       </c>
       <c r="G463" t="s">
         <v>27</v>
@@ -38049,22 +37999,22 @@
     </row>
     <row r="464" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A464" s="2" t="s">
-        <v>1398</v>
+        <v>1343</v>
       </c>
       <c r="B464" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C464" t="s">
-        <v>1347</v>
+        <v>113</v>
       </c>
       <c r="D464" t="s">
-        <v>1400</v>
+        <v>1486</v>
       </c>
       <c r="E464" t="s">
-        <v>1401</v>
+        <v>1486</v>
       </c>
       <c r="F464" t="s">
-        <v>1492</v>
+        <v>1402</v>
       </c>
       <c r="G464" t="s">
         <v>27</v>
@@ -38105,22 +38055,22 @@
     </row>
     <row r="465" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A465" s="2" t="s">
-        <v>1402</v>
+        <v>1344</v>
       </c>
       <c r="B465" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C465" t="s">
-        <v>1347</v>
+        <v>113</v>
       </c>
       <c r="D465" t="s">
-        <v>1399</v>
+        <v>114</v>
       </c>
       <c r="E465" t="s">
+        <v>1423</v>
+      </c>
+      <c r="F465" t="s">
         <v>1403</v>
-      </c>
-      <c r="F465" t="s">
-        <v>1493</v>
       </c>
       <c r="G465" t="s">
         <v>27</v>
@@ -38161,22 +38111,22 @@
     </row>
     <row r="466" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A466" s="2" t="s">
+        <v>1345</v>
+      </c>
+      <c r="B466" t="s">
+        <v>112</v>
+      </c>
+      <c r="C466" t="s">
+        <v>112</v>
+      </c>
+      <c r="D466" t="s">
+        <v>753</v>
+      </c>
+      <c r="E466" t="s">
+        <v>1494</v>
+      </c>
+      <c r="F466" t="s">
         <v>1404</v>
-      </c>
-      <c r="B466" t="s">
-        <v>1346</v>
-      </c>
-      <c r="C466" t="s">
-        <v>1405</v>
-      </c>
-      <c r="D466" t="s">
-        <v>1406</v>
-      </c>
-      <c r="E466" t="s">
-        <v>1407</v>
-      </c>
-      <c r="F466" t="s">
-        <v>1494</v>
       </c>
       <c r="G466" t="s">
         <v>27</v>
@@ -38217,22 +38167,22 @@
     </row>
     <row r="467" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A467" s="2" t="s">
-        <v>1408</v>
+        <v>1346</v>
       </c>
       <c r="B467" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C467" t="s">
+        <v>112</v>
+      </c>
+      <c r="D467" t="s">
+        <v>753</v>
+      </c>
+      <c r="E467" t="s">
+        <v>1495</v>
+      </c>
+      <c r="F467" t="s">
         <v>1405</v>
-      </c>
-      <c r="D467" t="s">
-        <v>1406</v>
-      </c>
-      <c r="E467" t="s">
-        <v>1409</v>
-      </c>
-      <c r="F467" t="s">
-        <v>1495</v>
       </c>
       <c r="G467" t="s">
         <v>27</v>
@@ -38273,22 +38223,22 @@
     </row>
     <row r="468" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A468" s="2" t="s">
-        <v>1410</v>
+        <v>1347</v>
       </c>
       <c r="B468" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C468" t="s">
-        <v>1405</v>
+        <v>112</v>
       </c>
       <c r="D468" t="s">
-        <v>1411</v>
+        <v>1460</v>
       </c>
       <c r="E468" t="s">
-        <v>1412</v>
+        <v>1465</v>
       </c>
       <c r="F468" t="s">
-        <v>1496</v>
+        <v>1406</v>
       </c>
       <c r="G468" t="s">
         <v>27</v>
@@ -38329,22 +38279,22 @@
     </row>
     <row r="469" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A469" s="2" t="s">
-        <v>1413</v>
+        <v>1348</v>
       </c>
       <c r="B469" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C469" t="s">
-        <v>1405</v>
+        <v>112</v>
       </c>
       <c r="D469" t="s">
-        <v>1414</v>
+        <v>1487</v>
       </c>
       <c r="E469" t="s">
-        <v>1415</v>
+        <v>1488</v>
       </c>
       <c r="F469" t="s">
-        <v>1497</v>
+        <v>1407</v>
       </c>
       <c r="G469" t="s">
         <v>27</v>
@@ -38385,22 +38335,22 @@
     </row>
     <row r="470" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A470" s="2" t="s">
-        <v>1416</v>
+        <v>1349</v>
       </c>
       <c r="B470" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C470" t="s">
-        <v>1405</v>
+        <v>112</v>
       </c>
       <c r="D470" t="s">
-        <v>1414</v>
+        <v>1487</v>
       </c>
       <c r="E470" t="s">
-        <v>1417</v>
+        <v>1489</v>
       </c>
       <c r="F470" t="s">
-        <v>1498</v>
+        <v>1408</v>
       </c>
       <c r="G470" t="s">
         <v>27</v>
@@ -38441,22 +38391,22 @@
     </row>
     <row r="471" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A471" s="2" t="s">
-        <v>1418</v>
+        <v>1350</v>
       </c>
       <c r="B471" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C471" t="s">
-        <v>1405</v>
+        <v>112</v>
       </c>
       <c r="D471" t="s">
-        <v>1414</v>
+        <v>1487</v>
       </c>
       <c r="E471" t="s">
-        <v>1419</v>
+        <v>1490</v>
       </c>
       <c r="F471" t="s">
-        <v>1499</v>
+        <v>1409</v>
       </c>
       <c r="G471" t="s">
         <v>27</v>
@@ -38497,22 +38447,22 @@
     </row>
     <row r="472" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A472" s="2" t="s">
-        <v>1420</v>
+        <v>1351</v>
       </c>
       <c r="B472" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C472" t="s">
-        <v>1405</v>
+        <v>112</v>
       </c>
       <c r="D472" t="s">
-        <v>1421</v>
+        <v>750</v>
       </c>
       <c r="E472" t="s">
-        <v>1422</v>
+        <v>1479</v>
       </c>
       <c r="F472" t="s">
-        <v>1500</v>
+        <v>1410</v>
       </c>
       <c r="G472" t="s">
         <v>27</v>
@@ -38553,22 +38503,22 @@
     </row>
     <row r="473" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A473" s="2" t="s">
-        <v>1423</v>
+        <v>1352</v>
       </c>
       <c r="B473" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C473" t="s">
-        <v>1405</v>
+        <v>112</v>
       </c>
       <c r="D473" t="s">
-        <v>1424</v>
+        <v>1441</v>
       </c>
       <c r="E473" t="s">
-        <v>1425</v>
+        <v>1447</v>
       </c>
       <c r="F473" t="s">
-        <v>1501</v>
+        <v>1411</v>
       </c>
       <c r="G473" t="s">
         <v>27</v>
@@ -38609,22 +38559,22 @@
     </row>
     <row r="474" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A474" s="2" t="s">
-        <v>1426</v>
+        <v>1353</v>
       </c>
       <c r="B474" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C474" t="s">
-        <v>1405</v>
+        <v>112</v>
       </c>
       <c r="D474" t="s">
-        <v>1427</v>
+        <v>1450</v>
       </c>
       <c r="E474" t="s">
-        <v>1428</v>
+        <v>1451</v>
       </c>
       <c r="F474" t="s">
-        <v>1502</v>
+        <v>1412</v>
       </c>
       <c r="G474" t="s">
         <v>27</v>
@@ -38665,22 +38615,22 @@
     </row>
     <row r="475" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A475" s="2" t="s">
-        <v>1429</v>
+        <v>1354</v>
       </c>
       <c r="B475" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C475" t="s">
-        <v>1405</v>
+        <v>112</v>
       </c>
       <c r="D475" t="s">
-        <v>1421</v>
+        <v>750</v>
       </c>
       <c r="E475" t="s">
-        <v>1430</v>
+        <v>1480</v>
       </c>
       <c r="F475" t="s">
-        <v>1503</v>
+        <v>1413</v>
       </c>
       <c r="G475" t="s">
         <v>27</v>
@@ -38721,22 +38671,22 @@
     </row>
     <row r="476" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A476" s="2" t="s">
-        <v>1431</v>
+        <v>1355</v>
       </c>
       <c r="B476" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C476" t="s">
-        <v>1405</v>
+        <v>112</v>
       </c>
       <c r="D476" t="s">
-        <v>1432</v>
+        <v>1471</v>
       </c>
       <c r="E476" t="s">
-        <v>1433</v>
+        <v>1481</v>
       </c>
       <c r="F476" t="s">
-        <v>1504</v>
+        <v>1414</v>
       </c>
       <c r="G476" t="s">
         <v>27</v>
@@ -38777,22 +38727,22 @@
     </row>
     <row r="477" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A477" s="2" t="s">
-        <v>1434</v>
+        <v>1356</v>
       </c>
       <c r="B477" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C477" t="s">
-        <v>1405</v>
+        <v>112</v>
       </c>
       <c r="D477" t="s">
-        <v>1432</v>
+        <v>1471</v>
       </c>
       <c r="E477" t="s">
-        <v>1435</v>
+        <v>1482</v>
       </c>
       <c r="F477" t="s">
-        <v>1505</v>
+        <v>1415</v>
       </c>
       <c r="G477" t="s">
         <v>27</v>
@@ -38833,22 +38783,22 @@
     </row>
     <row r="478" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A478" s="2" t="s">
-        <v>1436</v>
+        <v>1357</v>
       </c>
       <c r="B478" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C478" t="s">
-        <v>1405</v>
+        <v>112</v>
       </c>
       <c r="D478" t="s">
-        <v>1411</v>
+        <v>1460</v>
       </c>
       <c r="E478" t="s">
-        <v>1437</v>
+        <v>1466</v>
       </c>
       <c r="F478" t="s">
-        <v>1506</v>
+        <v>1416</v>
       </c>
       <c r="G478" t="s">
         <v>27</v>
@@ -38889,22 +38839,22 @@
     </row>
     <row r="479" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A479" s="2" t="s">
-        <v>1438</v>
+        <v>1358</v>
       </c>
       <c r="B479" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C479" t="s">
-        <v>1405</v>
+        <v>112</v>
       </c>
       <c r="D479" t="s">
-        <v>1414</v>
+        <v>1487</v>
       </c>
       <c r="E479" t="s">
-        <v>1439</v>
+        <v>1491</v>
       </c>
       <c r="F479" t="s">
-        <v>1507</v>
+        <v>1417</v>
       </c>
       <c r="G479" t="s">
         <v>27</v>
@@ -38945,22 +38895,22 @@
     </row>
     <row r="480" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A480" s="2" t="s">
-        <v>1440</v>
+        <v>1359</v>
       </c>
       <c r="B480" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C480" t="s">
-        <v>1405</v>
+        <v>112</v>
       </c>
       <c r="D480" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="E480" t="s">
-        <v>1442</v>
+        <v>1448</v>
       </c>
       <c r="F480" t="s">
-        <v>1508</v>
+        <v>1418</v>
       </c>
       <c r="G480" t="s">
         <v>27</v>
@@ -39001,22 +38951,22 @@
     </row>
     <row r="481" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A481" s="2" t="s">
-        <v>1443</v>
+        <v>1360</v>
       </c>
       <c r="B481" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C481" t="s">
-        <v>1405</v>
+        <v>112</v>
       </c>
       <c r="D481" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="E481" t="s">
-        <v>1444</v>
+        <v>1483</v>
       </c>
       <c r="F481" t="s">
-        <v>1509</v>
+        <v>1419</v>
       </c>
       <c r="G481" t="s">
         <v>27</v>
@@ -39057,22 +39007,22 @@
     </row>
     <row r="482" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A482" s="2" t="s">
-        <v>1445</v>
+        <v>1361</v>
       </c>
       <c r="B482" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C482" t="s">
-        <v>1405</v>
+        <v>112</v>
       </c>
       <c r="D482" t="s">
-        <v>1446</v>
+        <v>1427</v>
       </c>
       <c r="E482" t="s">
-        <v>1447</v>
+        <v>1426</v>
       </c>
       <c r="F482" t="s">
-        <v>1510</v>
+        <v>1420</v>
       </c>
       <c r="G482" t="s">
         <v>27</v>
@@ -39113,22 +39063,22 @@
     </row>
     <row r="483" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A483" s="2" t="s">
-        <v>1448</v>
+        <v>1362</v>
       </c>
       <c r="B483" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C483" t="s">
-        <v>1449</v>
+        <v>817</v>
       </c>
       <c r="D483" t="s">
-        <v>1450</v>
+        <v>817</v>
       </c>
       <c r="E483" t="s">
-        <v>1451</v>
+        <v>1492</v>
       </c>
       <c r="F483" t="s">
-        <v>1511</v>
+        <v>1421</v>
       </c>
       <c r="G483" t="s">
         <v>27</v>
@@ -39169,22 +39119,22 @@
     </row>
     <row r="484" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A484" s="2" t="s">
-        <v>1452</v>
+        <v>1363</v>
       </c>
       <c r="B484" t="s">
-        <v>1346</v>
+        <v>112</v>
       </c>
       <c r="C484" t="s">
-        <v>1449</v>
+        <v>817</v>
       </c>
       <c r="D484" t="s">
-        <v>1450</v>
+        <v>817</v>
       </c>
       <c r="E484" t="s">
-        <v>1453</v>
+        <v>1493</v>
       </c>
       <c r="F484" t="s">
-        <v>1512</v>
+        <v>1422</v>
       </c>
       <c r="G484" t="s">
         <v>27</v>

</xml_diff>